<commit_message>
- Fixed requirements.txt - Fixed test_results
</commit_message>
<xml_diff>
--- a/B0005/models/lstm/test_results_B0005.xlsx
+++ b/B0005/models/lstm/test_results_B0005.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardodalronco/Documents/Università degli studi Guglielmo Marconi/Laurea/Progetto/Progetti/battery_LSTM_explainability/B0005/models/lstm/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6204BB2-A26D-8247-997D-BF9C607F6D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -28,17 +34,17 @@
     <t>RMSE</t>
   </si>
   <si>
-    <t>MAPE (%)</t>
+    <t>MAE</t>
   </si>
   <si>
-    <t>MAE</t>
+    <t>MAPE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,17 +77,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -119,7 +133,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -153,6 +167,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -187,9 +202,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -362,14 +378,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G167"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,13 +401,13 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1.846327249719927</v>
       </c>
@@ -397,91 +415,91 @@
         <v>1.843129515647888</v>
       </c>
       <c r="D2">
-        <v>0.000116697987118916</v>
+        <v>1.16697987118916E-4</v>
       </c>
       <c r="E2">
-        <v>0.01080268425526341</v>
+        <v>1.0802684255263409E-2</v>
       </c>
       <c r="F2">
-        <v>0.01080268425526341</v>
+        <v>3.61033685069918E-3</v>
       </c>
       <c r="G2">
-        <v>0.005612305273368351</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>5.6123052733683511E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1.835349194223408</v>
+        <v>1.8353491942234079</v>
       </c>
       <c r="B3">
         <v>1.84416127204895</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1.835262527582113</v>
+        <v>1.8352625275821131</v>
       </c>
       <c r="B4">
         <v>1.833747863769531</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1.834645508212042</v>
+        <v>1.8346455082120421</v>
       </c>
       <c r="B5">
-        <v>1.834073305130005</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>1.8340733051300051</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1.835661660067549</v>
+        <v>1.8356616600675491</v>
       </c>
       <c r="B6">
         <v>1.833899617195129</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1.83514614292266</v>
+        <v>1.8351461429226601</v>
       </c>
       <c r="B7">
         <v>1.834136366844177</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>1.825756790566554</v>
+        <v>1.8257567905665539</v>
       </c>
       <c r="B8">
-        <v>1.833181023597717</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>1.8331810235977171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1.824773852989133</v>
+        <v>1.8247738529891331</v>
       </c>
       <c r="B9">
-        <v>1.825056433677673</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>1.8250564336776729</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1.824613268496936</v>
+        <v>1.8246132684969361</v>
       </c>
       <c r="B10">
-        <v>1.824341177940369</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>1.8243411779403691</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1.82461955268645</v>
+        <v>1.8246195526864499</v>
       </c>
       <c r="B11">
         <v>1.8245849609375</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1.814201935767392</v>
       </c>
@@ -489,87 +507,87 @@
         <v>1.825186014175415</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>1.813752157754905</v>
+        <v>1.8137521577549049</v>
       </c>
       <c r="B13">
         <v>1.813737630844116</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1.813440491473582</v>
       </c>
       <c r="B14">
-        <v>1.813647270202637</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>1.8136472702026369</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>1.80259800363065</v>
+        <v>1.8025980036306499</v>
       </c>
       <c r="B15">
         <v>1.812990784645081</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1.80210690024615</v>
+        <v>1.8021069002461501</v>
       </c>
       <c r="B16">
-        <v>1.804401993751526</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>1.8044019937515261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>1.802579500826209</v>
+        <v>1.8025795008262091</v>
       </c>
       <c r="B17">
-        <v>1.804433703422546</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>1.8044337034225459</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>1.80306831428341</v>
+        <v>1.8030683142834101</v>
       </c>
       <c r="B18">
         <v>1.805072426795959</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>1.802777624719604</v>
+        <v>1.8027776247196039</v>
       </c>
       <c r="B19">
         <v>1.805311322212219</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>1.847025994932919</v>
+        <v>1.8470259949329191</v>
       </c>
       <c r="B20">
         <v>1.804645776748657</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>1.847417311283644</v>
+        <v>1.8474173112836441</v>
       </c>
       <c r="B21">
         <v>1.843058228492737</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1.836177421347895</v>
       </c>
       <c r="B22">
-        <v>1.842184066772461</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>1.8421840667724609</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1.825780747577624</v>
       </c>
@@ -577,55 +595,55 @@
         <v>1.833349823951721</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1.825113643507837</v>
       </c>
       <c r="B24">
-        <v>1.825590014457703</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>1.8255900144577031</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1.825581504220376</v>
       </c>
       <c r="B25">
-        <v>1.824235916137695</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>1.8242359161376951</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>1.814031127508391</v>
+        <v>1.8140311275083909</v>
       </c>
       <c r="B26">
-        <v>1.826310157775879</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>1.8263101577758789</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>1.814769194115894</v>
+        <v>1.8147691941158941</v>
       </c>
       <c r="B27">
-        <v>1.815775036811829</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>1.8157750368118291</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>1.813969388710352</v>
+        <v>1.8139693887103521</v>
       </c>
       <c r="B28">
         <v>1.815732479095459</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1.802765665167823</v>
       </c>
       <c r="B29">
-        <v>1.815941095352173</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>1.8159410953521731</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1.804077040117352</v>
       </c>
@@ -633,7 +651,7 @@
         <v>1.805485725402832</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1.851802551670449</v>
       </c>
@@ -641,31 +659,31 @@
         <v>1.805634498596191</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>1.830703845673943</v>
+        <v>1.8307038456739431</v>
       </c>
       <c r="B32">
         <v>1.823072552680969</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1.819904108950127</v>
+        <v>1.8199041089501271</v>
       </c>
       <c r="B33">
         <v>1.819385409355164</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1.809307963702852</v>
       </c>
       <c r="B34">
-        <v>1.809592962265015</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>1.8095929622650151</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1.80460990458052</v>
       </c>
@@ -673,31 +691,31 @@
         <v>1.799643754959106</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1.799377065197219</v>
       </c>
       <c r="B36">
-        <v>1.796690225601196</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>1.7966902256011961</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>1.788443233537046</v>
+        <v>1.7884432335370459</v>
       </c>
       <c r="B37">
-        <v>1.788967251777649</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>1.7889672517776489</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>1.782923048425272</v>
+        <v>1.7829230484252721</v>
       </c>
       <c r="B38">
         <v>1.779675960540771</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1.773033715801829</v>
       </c>
@@ -705,15 +723,15 @@
         <v>1.776176452636719</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>1.773037755078937</v>
+        <v>1.7730377550789369</v>
       </c>
       <c r="B40">
         <v>1.766424775123596</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1.767872110666205</v>
       </c>
@@ -721,39 +739,39 @@
         <v>1.765361547470093</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>1.762315070409309</v>
+        <v>1.7623150704093089</v>
       </c>
       <c r="B42">
         <v>1.758647203445435</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>1.767617292493845</v>
+        <v>1.7676172924938449</v>
       </c>
       <c r="B43">
         <v>1.753227710723877</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1.762668359743147</v>
       </c>
       <c r="B44">
-        <v>1.759304046630859</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>1.7593040466308589</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>1.751730487066414</v>
+        <v>1.7517304870664141</v>
       </c>
       <c r="B45">
         <v>1.753856420516968</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1.741849604796001</v>
       </c>
@@ -761,7 +779,7 @@
         <v>1.744993329048157</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1.736091351184714</v>
       </c>
@@ -769,31 +787,31 @@
         <v>1.736818909645081</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1.793624014857361</v>
       </c>
       <c r="B48">
-        <v>1.730167746543884</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>1.7301677465438841</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1.783189022327327</v>
       </c>
       <c r="B49">
-        <v>1.783995270729065</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>1.7839952707290649</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>1.767364207627896</v>
+        <v>1.7673642076278959</v>
       </c>
       <c r="B50">
         <v>1.766898393630981</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1.757017785035307</v>
       </c>
@@ -801,63 +819,63 @@
         <v>1.755348682403564</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1.746870617983791</v>
       </c>
       <c r="B52">
-        <v>1.748619318008423</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>1.7486193180084231</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>1.741717250745714</v>
+        <v>1.7417172507457139</v>
       </c>
       <c r="B53">
         <v>1.738293528556824</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>1.736422505647819</v>
+        <v>1.7364225056478191</v>
       </c>
       <c r="B54">
-        <v>1.734589338302612</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>1.7345893383026121</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>1.726321723923583</v>
+        <v>1.7263217239235831</v>
       </c>
       <c r="B55">
         <v>1.727563142776489</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1.715806538933013</v>
       </c>
       <c r="B56">
-        <v>1.718408823013306</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
+        <v>1.7184088230133061</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>1.710533351135192</v>
+        <v>1.7105333511351919</v>
       </c>
       <c r="B57">
         <v>1.707924604415894</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>1.706014499648521</v>
+        <v>1.7060144996485209</v>
       </c>
       <c r="B58">
-        <v>1.703414559364319</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <v>1.7034145593643191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1.700311027264259</v>
       </c>
@@ -865,23 +883,23 @@
         <v>1.698906302452087</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1.694579860179789</v>
       </c>
       <c r="B60">
-        <v>1.691055774688721</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+        <v>1.6910557746887209</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>1.684902908660929</v>
+        <v>1.6849029086609291</v>
       </c>
       <c r="B61">
-        <v>1.686036825180054</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+        <v>1.6860368251800539</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1.674474159115972</v>
       </c>
@@ -889,7 +907,7 @@
         <v>1.67900550365448</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1.67456924798791</v>
       </c>
@@ -897,47 +915,47 @@
         <v>1.668604850769043</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>1.663716375981405</v>
+        <v>1.6637163759814051</v>
       </c>
       <c r="B64">
-        <v>1.667405605316162</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
+        <v>1.6674056053161621</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>1.659013868748246</v>
+        <v>1.6590138687482461</v>
       </c>
       <c r="B65">
         <v>1.654636144638062</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1.653854057333501</v>
       </c>
       <c r="B66">
-        <v>1.651858568191528</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
+        <v>1.6518585681915281</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1.642653782130131</v>
       </c>
       <c r="B67">
-        <v>1.647904276847839</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
+        <v>1.6479042768478389</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1.63785784302237</v>
       </c>
       <c r="B68">
-        <v>1.636557698249817</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
+        <v>1.6365576982498169</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1.632735040709911</v>
       </c>
@@ -945,31 +963,31 @@
         <v>1.632117033004761</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>1.627752891553362</v>
+        <v>1.6277528915533619</v>
       </c>
       <c r="B70">
         <v>1.626795887947083</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>1.622125485521159</v>
+        <v>1.6221254855211591</v>
       </c>
       <c r="B71">
         <v>1.622897624969482</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>1.611325660376585</v>
+        <v>1.6113256603765851</v>
       </c>
       <c r="B72">
         <v>1.615630984306335</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1.606563139748838</v>
       </c>
@@ -977,7 +995,7 @@
         <v>1.605144262313843</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1.601514223391759</v>
       </c>
@@ -985,47 +1003,47 @@
         <v>1.600645780563354</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>1.590369231400328</v>
+        <v>1.5903692314003279</v>
       </c>
       <c r="B75">
         <v>1.595348715782166</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>1.585788996824221</v>
+        <v>1.5857889968242209</v>
       </c>
       <c r="B76">
         <v>1.58467173576355</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>1.584943070737412</v>
+        <v>1.5849430707374119</v>
       </c>
       <c r="B77">
         <v>1.580960154533386</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>1.595526389249594</v>
+        <v>1.5955263892495939</v>
       </c>
       <c r="B78">
         <v>1.580597996711731</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>1.574730174780104</v>
+        <v>1.5747301747801039</v>
       </c>
       <c r="B79">
-        <v>1.586966633796692</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
+        <v>1.5869666337966919</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1.564901995093795</v>
       </c>
@@ -1033,7 +1051,7 @@
         <v>1.569509029388428</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1.559765947337036</v>
       </c>
@@ -1041,7 +1059,7 @@
         <v>1.561440110206604</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1.559481566818423</v>
       </c>
@@ -1049,15 +1067,15 @@
         <v>1.556968569755554</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>1.55468935359061</v>
+        <v>1.5546893535906099</v>
       </c>
       <c r="B83">
-        <v>1.553449630737305</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
+        <v>1.5534496307373049</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1.548874107989042</v>
       </c>
@@ -1065,31 +1083,31 @@
         <v>1.546867251396179</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>1.538236598942558</v>
+        <v>1.5382365989425579</v>
       </c>
       <c r="B85">
         <v>1.54213559627533</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>1.527914258251028</v>
+        <v>1.5279142582510279</v>
       </c>
       <c r="B86">
         <v>1.533333897590637</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>1.528525262975645</v>
+        <v>1.5285252629756449</v>
       </c>
       <c r="B87">
         <v>1.523552775382996</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1.522647325284378</v>
       </c>
@@ -1097,79 +1115,79 @@
         <v>1.523605585098267</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>1.517485993848987</v>
+        <v>1.5174859938489871</v>
       </c>
       <c r="B89">
-        <v>1.515590310096741</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
+        <v>1.5155903100967409</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1.563849144674442</v>
       </c>
       <c r="B90">
-        <v>1.510130167007446</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
+        <v>1.5101301670074461</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1.548091524776779</v>
       </c>
       <c r="B91">
-        <v>1.554087996482849</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
+        <v>1.5540879964828489</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>1.532375563186859</v>
       </c>
       <c r="B92">
-        <v>1.538744807243347</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
+        <v>1.5387448072433469</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1.52695282684897</v>
       </c>
       <c r="B93">
-        <v>1.524215579032898</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
+        <v>1.5242155790328979</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>1.516957301713633</v>
+        <v>1.5169573017136331</v>
       </c>
       <c r="B94">
-        <v>1.519638895988464</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
+        <v>1.5196388959884639</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>1.511897596014269</v>
+        <v>1.5118975960142691</v>
       </c>
       <c r="B95">
-        <v>1.510505080223083</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
+        <v>1.5105050802230831</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>1.50656389606811</v>
       </c>
       <c r="B96">
-        <v>1.505263805389404</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
+        <v>1.5052638053894041</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>1.501545352667136</v>
+        <v>1.5015453526671361</v>
       </c>
       <c r="B97">
-        <v>1.499523043632507</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
+        <v>1.4995230436325071</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>1.490844405040024</v>
       </c>
@@ -1177,23 +1195,23 @@
         <v>1.495110750198364</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>1.485868384561201</v>
+        <v>1.4858683845612011</v>
       </c>
       <c r="B99">
-        <v>1.483890891075134</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
+        <v>1.4838908910751341</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>1.480413677976106</v>
+        <v>1.4804136779761059</v>
       </c>
       <c r="B100">
         <v>1.478768110275269</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>1.475209586903163</v>
       </c>
@@ -1201,71 +1219,71 @@
         <v>1.473375797271729</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>1.485903598830402</v>
+        <v>1.4859035988304019</v>
       </c>
       <c r="B102">
-        <v>1.46878457069397</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
+        <v>1.4687845706939699</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>1.49609182981367</v>
+        <v>1.4960918298136701</v>
       </c>
       <c r="B103">
         <v>1.4791419506073</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>1.480800594692898</v>
+        <v>1.4808005946928979</v>
       </c>
       <c r="B104">
-        <v>1.485689401626587</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
+        <v>1.4856894016265869</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>1.469754326846682</v>
+        <v>1.4697543268466819</v>
       </c>
       <c r="B105">
-        <v>1.470800280570984</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
+        <v>1.4708002805709841</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>1.453901227484593</v>
+        <v>1.4539012274845931</v>
       </c>
       <c r="B106">
         <v>1.461529135704041</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>1.454146206723569</v>
+        <v>1.4541462067235691</v>
       </c>
       <c r="B107">
-        <v>1.446455955505371</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
+        <v>1.4464559555053711</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>1.455023751906683</v>
+        <v>1.4550237519066831</v>
       </c>
       <c r="B108">
-        <v>1.446651577949524</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
+        <v>1.4466515779495239</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>1.449042163761236</v>
+        <v>1.4490421637612361</v>
       </c>
       <c r="B109">
-        <v>1.446683645248413</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
+        <v>1.4466836452484131</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>1.438670937148057</v>
       </c>
@@ -1273,15 +1291,15 @@
         <v>1.438758373260498</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>1.433445432156979</v>
+        <v>1.4334454321569789</v>
       </c>
       <c r="B111">
-        <v>1.429722309112549</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
+        <v>1.4297223091125491</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>1.43339589008381</v>
       </c>
@@ -1289,183 +1307,183 @@
         <v>1.425921678543091</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>1.42806487344776</v>
+        <v>1.4280648734477599</v>
       </c>
       <c r="B113">
         <v>1.425201892852783</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>1.422920318174119</v>
       </c>
       <c r="B114">
-        <v>1.417342662811279</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2">
+        <v>1.4173426628112791</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>1.417429032731308</v>
+        <v>1.4174290327313079</v>
       </c>
       <c r="B115">
         <v>1.412892699241638</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>1.412409228794446</v>
+        <v>1.4124092287944461</v>
       </c>
       <c r="B116">
         <v>1.408779382705688</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>1.412578792940193</v>
       </c>
       <c r="B117">
-        <v>1.405397057533264</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
+        <v>1.4053970575332639</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>1.40759837314699</v>
+        <v>1.4075983731469901</v>
       </c>
       <c r="B118">
         <v>1.404261112213135</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119">
-        <v>1.433392048522148</v>
+        <v>1.4333920485221481</v>
       </c>
       <c r="B119">
-        <v>1.397283315658569</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
+        <v>1.3972833156585689</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>1.438255017679291</v>
       </c>
       <c r="B120">
-        <v>1.422531604766846</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
+        <v>1.4225316047668459</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>1.417354717448553</v>
       </c>
       <c r="B121">
-        <v>1.426716446876526</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
+        <v>1.4267164468765261</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>1.406981663677643</v>
+        <v>1.4069816636776431</v>
       </c>
       <c r="B122">
         <v>1.407206654548645</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>1.401203778358763</v>
       </c>
       <c r="B123">
-        <v>1.399205446243286</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
+        <v>1.3992054462432859</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>1.396700823272633</v>
       </c>
       <c r="B124">
-        <v>1.393993854522705</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
+        <v>1.3939938545227051</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>1.391284788852726</v>
       </c>
       <c r="B125">
-        <v>1.389698624610901</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
+        <v>1.3896986246109011</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126">
-        <v>1.386228767797835</v>
+        <v>1.3862287677978351</v>
       </c>
       <c r="B126">
-        <v>1.384506344795227</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
+        <v>1.3845063447952271</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127">
-        <v>1.380436676197414</v>
+        <v>1.3804366761974141</v>
       </c>
       <c r="B127">
-        <v>1.379661321640015</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
+        <v>1.3796613216400151</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>1.375236415025622</v>
       </c>
       <c r="B128">
-        <v>1.374343514442444</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2">
+        <v>1.3743435144424441</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>1.370512802489501</v>
       </c>
       <c r="B129">
-        <v>1.37045693397522</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2">
+        <v>1.3704569339752199</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130">
-        <v>1.37050855662704</v>
+        <v>1.3705085566270401</v>
       </c>
       <c r="B130">
         <v>1.365161180496216</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>1.364735510868152</v>
       </c>
       <c r="B131">
-        <v>1.364866137504578</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2">
+        <v>1.3648661375045781</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132">
-        <v>1.375392016895762</v>
+        <v>1.3753920168957621</v>
       </c>
       <c r="B132">
-        <v>1.35964822769165</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2">
+        <v>1.3596482276916499</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>1.386111515153539</v>
       </c>
       <c r="B133">
-        <v>1.370548963546753</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2">
+        <v>1.3705489635467529</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134">
-        <v>1.369850003583894</v>
+        <v>1.3698500035838941</v>
       </c>
       <c r="B134">
-        <v>1.375987410545349</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2">
+        <v>1.3759874105453489</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>1.364782794926076</v>
       </c>
@@ -1473,7 +1491,7 @@
         <v>1.361950039863586</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>1.354322046625996</v>
       </c>
@@ -1481,7 +1499,7 @@
         <v>1.357760071754456</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>1.354641701837896</v>
       </c>
@@ -1489,47 +1507,47 @@
         <v>1.349058866500854</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138">
-        <v>1.354703921319241</v>
+        <v>1.3547039213192409</v>
       </c>
       <c r="B138">
-        <v>1.347945213317871</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2">
+        <v>1.3479452133178711</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>1.349314997503458</v>
       </c>
       <c r="B139">
-        <v>1.34609317779541</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2">
+        <v>1.3460931777954099</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140">
-        <v>1.344189193797055</v>
+        <v>1.3441891937970549</v>
       </c>
       <c r="B140">
-        <v>1.342244863510132</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2">
+        <v>1.3422448635101321</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>1.338991379069576</v>
       </c>
       <c r="B141">
-        <v>1.339233636856079</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2">
+        <v>1.3392336368560791</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142">
-        <v>1.338914523020697</v>
+        <v>1.3389145230206969</v>
       </c>
       <c r="B142">
         <v>1.334821224212646</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>1.334006675976166</v>
       </c>
@@ -1537,7 +1555,7 @@
         <v>1.33356249332428</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>1.328644430917491</v>
       </c>
@@ -1545,23 +1563,23 @@
         <v>1.327714681625366</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145">
-        <v>1.323170899227622</v>
+        <v>1.3231708992276221</v>
       </c>
       <c r="B145">
-        <v>1.324712038040161</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2">
+        <v>1.3247120380401609</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146">
-        <v>1.31816915884452</v>
+        <v>1.3181691588445199</v>
       </c>
       <c r="B146">
-        <v>1.320236206054688</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2">
+        <v>1.3202362060546879</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>1.318466443664033</v>
       </c>
@@ -1569,87 +1587,87 @@
         <v>1.316048145294189</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>1.318293040102702</v>
       </c>
       <c r="B148">
-        <v>1.31395149230957</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2">
+        <v>1.3139514923095701</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149">
-        <v>1.323872422244268</v>
+        <v>1.3238724222442679</v>
       </c>
       <c r="B149">
-        <v>1.314496040344238</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2">
+        <v>1.3144960403442381</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>1.360121676655478</v>
       </c>
       <c r="B150">
-        <v>1.319199562072754</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2">
+        <v>1.3191995620727539</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>1.339530686794735</v>
       </c>
       <c r="B151">
-        <v>1.353313326835632</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2">
+        <v>1.3533133268356321</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152">
-        <v>1.32902865651207</v>
+        <v>1.3290286565120699</v>
       </c>
       <c r="B152">
-        <v>1.333806872367859</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2">
+        <v>1.3338068723678591</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>1.323674127499896</v>
       </c>
       <c r="B153">
-        <v>1.324433088302612</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2">
+        <v>1.3244330883026121</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154">
-        <v>1.318633896753293</v>
+        <v>1.3186338967532929</v>
       </c>
       <c r="B154">
         <v>1.320472359657288</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155">
-        <v>1.313475132132427</v>
+        <v>1.3134751321324269</v>
       </c>
       <c r="B155">
         <v>1.315366268157959</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156">
-        <v>1.31320206344422</v>
+        <v>1.3132020634442201</v>
       </c>
       <c r="B156">
-        <v>1.31037175655365</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2">
+        <v>1.3103717565536499</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157">
-        <v>1.307795994694435</v>
+        <v>1.3077959946944351</v>
       </c>
       <c r="B157">
-        <v>1.310101866722107</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2">
+        <v>1.3101018667221069</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>1.303032918640592</v>
       </c>
@@ -1657,7 +1675,7 @@
         <v>1.30491042137146</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>1.303357355903821</v>
       </c>
@@ -1665,7 +1683,7 @@
         <v>1.300000786781311</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>1.303410043865564</v>
       </c>
@@ -1673,57 +1691,57 @@
         <v>1.300626397132874</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>1.297887080649571</v>
       </c>
       <c r="B161">
-        <v>1.300364375114441</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2">
+        <v>1.3003643751144409</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>1.29807350569189</v>
       </c>
       <c r="B162">
-        <v>1.294700264930725</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2">
+        <v>1.2947002649307251</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>1.293463613844243</v>
       </c>
       <c r="B163">
-        <v>1.295279145240784</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2">
+        <v>1.2952791452407839</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164">
-        <v>1.288003392619118</v>
+        <v>1.2880033926191179</v>
       </c>
       <c r="B164">
         <v>1.29102635383606</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165">
-        <v>1.287452522137941</v>
+        <v>1.2874525221379409</v>
       </c>
       <c r="B165">
-        <v>1.285238146781921</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2">
+        <v>1.2852381467819209</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166">
-        <v>1.309015364230735</v>
+        <v>1.3090153642307349</v>
       </c>
       <c r="B166">
         <v>1.28411853313446</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167">
-        <v>1.325079328642936</v>
+        <v>1.3250793286429361</v>
       </c>
       <c r="B167">
         <v>1.305723905563354</v>

</xml_diff>